<commit_message>
Add Doctor profile update API
</commit_message>
<xml_diff>
--- a/IKSANA_API_TESTING/Files/Iksana_API_Testing_Testcases_v0.1.xlsx
+++ b/IKSANA_API_TESTING/Files/Iksana_API_Testing_Testcases_v0.1.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5991" uniqueCount="1879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6002" uniqueCount="1879">
   <si>
     <t>Mavens i
 IKSANA
@@ -13915,7 +13915,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -14701,18 +14701,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8727272727273" defaultRowHeight="42" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7545454545455" style="29" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.7545454545455" style="29" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.2545454545455" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5" style="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.8727272727273" style="12" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.8727272727273" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.8727272727273" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="29" width="18.7545454545455" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="36.8727272727273" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="29" width="30.7545454545455" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.2545454545455" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="12" width="13.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="32.8727272727273" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="24.6272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="12" width="14.8727272727273" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.8727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:11">
@@ -15396,14 +15396,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.6272727272727" defaultRowHeight="39" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.25454545454545" style="12" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.6272727272727" style="29" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.6272727272727" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="12" width="7.25454545454545" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.8727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.6272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="32.6272727272727" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="29" width="15.6272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.3727272727273" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.6272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="1" customHeight="1" spans="1:11">
@@ -15897,14 +15897,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.6272727272727" defaultRowHeight="39" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.25454545454545" style="12" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.2545454545455" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.6272727272727" style="29" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.6272727272727" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="12" width="7.25454545454545" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.6272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.2545454545455" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="32.6272727272727" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="29" width="15.6272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.3727272727273" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.6272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="1" customHeight="1" spans="1:11">
@@ -17020,14 +17020,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7545454545455" defaultRowHeight="33" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="35.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.2545454545455" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7545454545455" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.7545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.3727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.7545454545455" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="35.3727272727273" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7545454545455" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.7545454545455" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.2545454545455" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.7545454545455" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:11">
@@ -17767,14 +17767,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7545454545455" defaultRowHeight="33" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.2545454545455" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7545454545455" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.7545454545455" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.8727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.7545454545455" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="32.1272727272727" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7545454545455" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.7545454545455" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.2545454545455" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.7545454545455" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="1" customHeight="1" spans="1:11">
@@ -19799,16 +19799,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="33" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="27.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="25.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.8727272727273" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="27.6272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.8727272727273" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.7545454545455" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.1272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.3727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.1272727272727" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="23.8727272727273" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="25.3727272727273" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.8727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="1" customHeight="1" spans="1:11">
@@ -20279,17 +20279,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25454545454545" defaultRowHeight="32.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.25454545454545" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.25454545454545" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.25454545454545" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="9.25454545454545" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.8727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="32.1272727272727" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.8727272727273" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.8727272727273" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.25454545454545" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="22.1272727272727" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="9.25454545454545" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="1" customHeight="1" spans="1:11">
@@ -20881,14 +20881,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="45" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="21.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.6272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="21.3727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.6272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.1272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.3727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.3727272727273" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.6272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="1" customHeight="1" spans="1:11">
@@ -21312,14 +21312,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="45" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="21.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6272727272727" style="12" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.6272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="21.3727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="12" width="17.6272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.1272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.3727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.3727272727273" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.6272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="1" customHeight="1" spans="1:11">
@@ -21711,14 +21711,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="45" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="28.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6272727272727" style="12" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.6272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="28.8727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="12" width="17.6272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.1272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.3727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.3727272727273" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.6272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="1" customHeight="1" spans="1:11">
@@ -22239,11 +22239,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="27.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.8727272727273" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.1272727272727" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.8727272727273" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.1272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="7" max="7" width="10.8727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:4">
@@ -23403,14 +23403,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="45" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="21.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6272727272727" style="12" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.6272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="21.6272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="12" width="17.6272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.1272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.3727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.3727272727273" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.6272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="1" customHeight="1" spans="1:11">
@@ -24005,14 +24005,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="45" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="21.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6272727272727" style="12" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.6272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="21.6272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="12" width="17.6272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.1272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.3727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.3727272727273" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.6272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="1" customHeight="1" spans="1:11">
@@ -24739,14 +24739,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="45" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="16.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6272727272727" style="12" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.6272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="16.6272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="12" width="17.6272727272727" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.1272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.3727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.3727272727273" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.6272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="1" customHeight="1" spans="1:11">
@@ -25409,18 +25409,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.75454545454545" style="9" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" style="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.3727272727273" style="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5" style="9" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.8727272727273" style="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.2545454545455" style="9" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.1272727272727" style="9" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.1272727272727" style="9" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.8727272727273" style="9" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.6272727272727" style="9" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="8.75454545454545" style="9" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="9" width="7.75454545454545" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="9" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="15" width="15.3727272727273" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="9" width="18.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="15" width="16.8727272727273" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="9" width="12.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="9" width="15.2545454545455" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="9" width="15.1272727272727" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="9" width="13.1272727272727" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="9" width="12.8727272727273" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="9" width="12.6272727272727" collapsed="true"/>
+    <col min="12" max="16384" style="9" width="8.75454545454545" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="1" ht="45" customHeight="1" spans="1:11">
@@ -26219,17 +26219,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="12" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.3727272727273" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="12" width="10.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.1272727272727" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.7545454545455" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.1272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.8727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.1272727272727" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.1272727272727" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.1272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="11.3727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="50.1" customHeight="1" spans="1:11">
@@ -26997,17 +26997,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="12" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.2545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.3727272727273" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="12" width="10.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.2545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.7545454545455" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.1272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.8727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.1272727272727" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.1272727272727" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.1272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="11.3727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="50.1" customHeight="1" spans="1:11">
@@ -27774,17 +27774,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="12" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.2545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.3727272727273" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="12" width="10.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.2545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.7545454545455" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.1272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.8727272727273" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.1272727272727" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.1272727272727" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.1272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="11.3727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="50.1" customHeight="1" spans="1:11">
@@ -28551,16 +28551,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="15.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.2545454545455" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.1272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="15.7545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.6272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.1272727272727" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.3727272727273" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.2545454545455" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.1272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="50.1" customHeight="1" spans="1:11">
@@ -29327,16 +29327,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="15.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.2545454545455" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.1272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="15.7545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.6272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.1272727272727" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.3727272727273" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.2545454545455" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.1272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="50.1" customHeight="1" spans="1:11">
@@ -30103,16 +30103,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="15.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.6272727272727" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.1272727272727" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.3727272727273" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.2545454545455" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.1272727272727" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="15.7545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.6272727272727" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.1272727272727" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.3727272727273" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.2545454545455" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.1272727272727" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="50.1" customHeight="1" spans="1:11">
@@ -30878,17 +30878,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8727272727273" defaultRowHeight="28" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.36363636363636" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.5454545454545" style="9" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="76.9090909090909" style="51" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.7545454545455" style="29" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.8181818181818" style="12" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5" style="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.6272727272727" style="39" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.8727272727273" style="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="6.36363636363636" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.6363636363636" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="9" width="28.5454545454545" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="51" width="76.9090909090909" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="29" width="30.7545454545455" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="12" width="13.8181818181818" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="12" width="13.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="32.8727272727273" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="39" width="24.6272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="12" width="14.8727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" customHeight="1" spans="1:11">
@@ -32704,17 +32704,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8727272727273" defaultRowHeight="28" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.36363636363636" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.9090909090909" style="9" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="76.9090909090909" style="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.8181818181818" style="29" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.8181818181818" style="12" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5" style="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.6272727272727" style="39" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.8727272727273" style="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="6.36363636363636" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.6363636363636" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="9" width="29.9090909090909" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="38" width="76.9090909090909" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="29" width="31.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="12" width="13.8181818181818" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="12" width="13.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="32.8727272727273" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="39" width="24.6272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="12" width="14.8727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" customHeight="1" spans="1:11">
@@ -34139,17 +34139,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8727272727273" defaultRowHeight="28" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.36363636363636" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.9090909090909" style="9" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="76.9090909090909" style="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.8181818181818" style="29" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.8181818181818" style="12" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5" style="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.6272727272727" style="39" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.8727272727273" style="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="6.36363636363636" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.6363636363636" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="9" width="29.9090909090909" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="38" width="76.9090909090909" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="29" width="31.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="12" width="13.8181818181818" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="12" width="13.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="32.8727272727273" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="39" width="24.6272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="12" width="14.8727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" customHeight="1" spans="1:11">
@@ -35561,17 +35561,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8727272727273" defaultRowHeight="28" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.36363636363636" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.7272727272727" style="9" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="76.9090909090909" style="51" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.8181818181818" style="29" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.8181818181818" style="12" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5" style="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.6272727272727" style="39" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.8727272727273" style="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="6.36363636363636" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.6363636363636" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="9" width="32.7272727272727" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="51" width="76.9090909090909" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="29" width="31.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="12" width="13.8181818181818" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="12" width="13.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="32.8727272727273" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="39" width="24.6272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="12" width="14.8727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" customHeight="1" spans="1:11">
@@ -37394,17 +37394,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8727272727273" defaultRowHeight="28" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.36363636363636" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.9090909090909" style="9" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="74.8181818181818" style="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.8181818181818" style="29" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.8181818181818" style="12" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5" style="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.8727272727273" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.6272727272727" style="39" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.8727272727273" style="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="6.36363636363636" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.2727272727273" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="9" width="29.9090909090909" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="38" width="74.8181818181818" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="29" width="31.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="12" width="13.8181818181818" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="12" width="13.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="32.8727272727273" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="39" width="24.6272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="12" width="14.8727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" customHeight="1" spans="1:11">
@@ -38694,17 +38694,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8727272727273" defaultRowHeight="28" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.36363636363636" customWidth="1"/>
-    <col min="2" max="2" width="18.7545454545455" customWidth="1"/>
-    <col min="3" max="3" width="15.2727272727273" customWidth="1"/>
-    <col min="4" max="4" width="29.9090909090909" style="9" customWidth="1"/>
-    <col min="5" max="5" width="74.8181818181818" style="38" customWidth="1"/>
-    <col min="6" max="6" width="31.8181818181818" style="29" customWidth="1"/>
-    <col min="7" max="7" width="13.8181818181818" style="12" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="12" customWidth="1"/>
-    <col min="9" max="9" width="32.8727272727273" customWidth="1"/>
-    <col min="10" max="10" width="24.6272727272727" style="39" customWidth="1"/>
-    <col min="11" max="11" width="14.8727272727273" style="12" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.36363636363636" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7545454545455" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.2727272727273" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="9" width="29.9090909090909" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="38" width="74.8181818181818" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="29" width="31.8181818181818" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="12" width="13.8181818181818" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="12" width="13.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="32.8727272727273" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="39" width="24.6272727272727" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="12" width="14.8727272727273" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" customHeight="1" spans="1:11">

</xml_diff>

<commit_message>
update caregiver profile details
</commit_message>
<xml_diff>
--- a/IKSANA_API_TESTING/Files/Iksana_API_Testing_Testcases_v0.1.xlsx
+++ b/IKSANA_API_TESTING/Files/Iksana_API_Testing_Testcases_v0.1.xlsx
@@ -2573,6 +2573,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Update Caregiver Profile:</t>
     </r>
     <r>
@@ -32732,7 +32740,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="H1 K3:K15 K1" listDataValidation="1"/>
+    <ignoredError sqref="K1 K3:K15 H1" listDataValidation="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -38722,7 +38730,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="G1:H1 K1" listDataValidation="1"/>
+    <ignoredError sqref="K1 G1:H1" listDataValidation="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -38733,7 +38741,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8727272727273" defaultRowHeight="28" customHeight="1"/>
@@ -40060,10 +40068,10 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G25 G26:G31 G32:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G$1:G$1048576">
       <formula1>"GET,POST,PUT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H25 H26:H31 H32:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H$1:H$1048576">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K$1:K$1048576">

</xml_diff>

<commit_message>
small changes add on profile excel files
</commit_message>
<xml_diff>
--- a/IKSANA_API_TESTING/Files/Iksana_API_Testing_Testcases_v0.1.xlsx
+++ b/IKSANA_API_TESTING/Files/Iksana_API_Testing_Testcases_v0.1.xlsx
@@ -2614,6 +2614,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Update Veteran Profile:</t>
     </r>
     <r>
@@ -38770,8 +38778,8 @@
   <sheetPr/>
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8727272727273" defaultRowHeight="28" customHeight="1"/>

</xml_diff>